<commit_message>
khaeril bayar april mei
</commit_message>
<xml_diff>
--- a/kas asrama.xlsx
+++ b/kas asrama.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WORK\Asrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="106">
   <si>
     <t>kas asrama</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>75 (tf)</t>
+  </si>
+  <si>
+    <t>75(tf)</t>
   </si>
 </sst>
 </file>
@@ -467,11 +470,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,13 +807,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1509,7 +1512,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1574,7 +1577,12 @@
       <c r="E2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="J2" t="s">
         <v>34</v>
       </c>
@@ -1618,7 +1626,7 @@
       <c r="F3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J3" t="s">
@@ -1734,7 +1742,7 @@
       <c r="F7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J7" t="s">

</xml_diff>

<commit_message>
sholeh bayar 125, david 75, sidiq 75
</commit_message>
<xml_diff>
--- a/kas asrama.xlsx
+++ b/kas asrama.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WORK\Asrama\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B03ABC-F77D-45A2-AF04-3880A637ED7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="_" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="107">
   <si>
     <t>kas asrama</t>
   </si>
@@ -349,12 +350,15 @@
   </si>
   <si>
     <t>75(tf)</t>
+  </si>
+  <si>
+    <t>v (50 tf)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -789,7 +793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1508,11 +1512,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1603,8 +1607,8 @@
         <v>98</v>
       </c>
       <c r="P2">
-        <f>875000+75000 + 425000</f>
-        <v>1375000</v>
+        <f>875000+75000 + 425000 + 75000*3 + 125000</f>
+        <v>1725000</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -1718,7 +1722,9 @@
       <c r="E6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="J6" t="s">
         <v>87</v>
       </c>
@@ -1859,7 +1865,7 @@
       </c>
       <c r="P12">
         <f>N10-P1-P2-C28-D28-E28-F28</f>
-        <v>187250</v>
+        <v>-162750</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -1881,6 +1887,9 @@
       <c r="F13" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="G13" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1906,7 +1915,7 @@
       </c>
       <c r="P14">
         <f>2100000-P12-K17</f>
-        <v>1862750</v>
+        <v>2212750</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
@@ -2114,10 +2123,15 @@
       <c r="D24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="4">
-        <v>100</v>
-      </c>
-      <c r="F24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -2215,6 +2229,9 @@
       </c>
       <c r="F29" s="9" t="s">
         <v>91</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>